<commit_message>
new final data raw + processed
</commit_message>
<xml_diff>
--- a/Final/HUHF-IOT-TEST_005-CSV_POST_PROC/HUHF-IOT-TEST_005-CSV_COND1/cond1_loc0_processed.xlsx
+++ b/Final/HUHF-IOT-TEST_005-CSV_POST_PROC/HUHF-IOT-TEST_005-CSV_COND1/cond1_loc0_processed.xlsx
@@ -384,7 +384,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.00015199999999993</v>
+        <v>0.0001410000000001688</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -392,7 +392,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.0001419999999998645</v>
+        <v>0.0001319999999997989</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -400,7 +400,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.0001210000000000377</v>
+        <v>0.000135999999999914</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -408,7 +408,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.001794999999999991</v>
+        <v>0.005838000000000232</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -416,7 +416,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.007608999999999977</v>
+        <v>0.02350299999999983</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -424,7 +424,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>7.100000000015427E-05</v>
+        <v>0.0001189999999997582</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -432,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.002024000000000026</v>
+        <v>0.009040999999999855</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -440,7 +440,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.004275000000000251</v>
+        <v>9.900000000007125E-05</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -448,7 +448,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.0001539999999997654</v>
+        <v>0.000135999999999914</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -456,7 +456,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.0001360000000003581</v>
+        <v>0.0133289999999997</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -464,7 +464,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.01326800000000006</v>
+        <v>0.002038999999999902</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -472,7 +472,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.01233799999999974</v>
+        <v>0.0234709999999998</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -480,7 +480,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.005167000000000144</v>
+        <v>0.00510300000000008</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -488,7 +488,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.002067000000000263</v>
+        <v>0.02921599999999991</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -496,7 +496,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5579400000000003</v>
+        <v>0.5820000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -504,7 +504,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.0815030000000001</v>
+        <v>0.04435300000000009</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -512,7 +512,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.04706900000000003</v>
+        <v>0.0439449999999999</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -520,7 +520,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.006917999999999758</v>
+        <v>0.04438699999999995</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -528,7 +528,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.03493499999999994</v>
+        <v>0.04941099999999965</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -536,7 +536,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.06318299999999999</v>
+        <v>0.04439800000000016</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -544,7 +544,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.007025999999999755</v>
+        <v>0.04435099999999981</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -552,7 +552,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.01806099999999988</v>
+        <v>0.04454399999999969</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -560,7 +560,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.05057699999999965</v>
+        <v>0.04438299999999984</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -568,7 +568,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.009025999999999534</v>
+        <v>0.04470000000000018</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -576,7 +576,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.03597300000000025</v>
+        <v>0.04435499999999948</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -584,7 +584,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.03403799999999979</v>
+        <v>0.03106600000000004</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -592,7 +592,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.02104799999999951</v>
+        <v>0.04437300000000022</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -600,7 +600,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.01499999999999968</v>
+        <v>0.04455100000000023</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -608,7 +608,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.07209500000000002</v>
+        <v>0.04443600000000014</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -616,7 +616,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.06032499999999974</v>
+        <v>0.0785619999999998</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -624,7 +624,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.01718799999999998</v>
+        <v>0.04461199999999987</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -632,7 +632,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.04432799999999926</v>
+        <v>0.04455900000000046</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -640,7 +640,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.03020699999999987</v>
+        <v>0.04436299999999971</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -648,7 +648,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.08329900000000023</v>
+        <v>0.04455999999999971</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -656,7 +656,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.08545099999999994</v>
+        <v>0.04429199999999955</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -664,7 +664,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.03922599999999932</v>
+        <v>0.04454599999999953</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -672,7 +672,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.03519699999999926</v>
+        <v>0.04449400000000026</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -680,7 +680,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.04451099999999997</v>
+        <v>0.04423199999999916</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -688,7 +688,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.04449499999999951</v>
+        <v>0.04445499999999925</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -696,7 +696,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.01106799999999986</v>
+        <v>0.0444110000000002</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -704,7 +704,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.02785299999999946</v>
+        <v>0.04409599999999969</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -712,7 +712,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.03500800000000037</v>
+        <v>0.04439200000000021</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -720,7 +720,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.04456500000000041</v>
+        <v>0.04438000000000031</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -728,7 +728,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.03102499999999964</v>
+        <v>0.04459700000000044</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -736,7 +736,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.06630799999999937</v>
+        <v>0.0444899999999997</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -744,7 +744,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.03498099999999926</v>
+        <v>0.04448600000000003</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -752,7 +752,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.04478800000000049</v>
+        <v>0.04405099999999962</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -760,7 +760,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.007089999999999819</v>
+        <v>0.04459800000000058</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -768,7 +768,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.04831200000000013</v>
+        <v>0.04437800000000003</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -776,7 +776,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.04434000000000005</v>
+        <v>0.04440299999999997</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -784,7 +784,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.06598299999999924</v>
+        <v>0.04450900000000058</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -792,7 +792,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.07447599999999976</v>
+        <v>0.04444500000000051</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -800,7 +800,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.04435000000000056</v>
+        <v>0.04423399999999944</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -808,7 +808,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.004220000000000113</v>
+        <v>0.04457999999999984</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -816,7 +816,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.01401599999999981</v>
+        <v>0.04442699999999977</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -824,7 +824,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.004058000000000561</v>
+        <v>0.04458399999999951</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -832,7 +832,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.04459899999999983</v>
+        <v>0.04446200000000022</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -840,7 +840,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.02002999999999933</v>
+        <v>0.04423499999999958</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -848,7 +848,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.04460599999999992</v>
+        <v>0.04457299999999975</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -856,7 +856,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.05353399999999997</v>
+        <v>0.04441899999999954</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -864,7 +864,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.01400899999999972</v>
+        <v>0.04442099999999982</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -872,7 +872,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.04996599999999951</v>
+        <v>0.008856999999999893</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -880,7 +880,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.06054000000000048</v>
+        <v>0.03004500000000032</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -888,7 +888,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.07934299999999972</v>
+        <v>0.04458499999999965</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -896,7 +896,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.051647</v>
+        <v>0.04441300000000048</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -904,7 +904,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.03302200000000077</v>
+        <v>0.04440499999999936</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -912,7 +912,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.01703600000000094</v>
+        <v>0.04443699999999939</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -920,7 +920,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.05819800000000086</v>
+        <v>0.05439900000000009</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -928,7 +928,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.05855500000000013</v>
+        <v>0.04466699999999957</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -936,7 +936,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.05199599999999904</v>
+        <v>0.04441600000000001</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -944,7 +944,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.05548199999999959</v>
+        <v>0.04423500000000047</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -952,7 +952,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.04438099999999956</v>
+        <v>0.04463100000000075</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -960,7 +960,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.03201699999999974</v>
+        <v>0.04443299999999972</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -968,7 +968,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.08954599999999857</v>
+        <v>0.04442799999999991</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -976,7 +976,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.04121299999999906</v>
+        <v>0.04444099999999906</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -984,7 +984,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.003027999999998698</v>
+        <v>0.04425600000000074</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -992,7 +992,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.03399500000000089</v>
+        <v>0.04445999999999906</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1000,7 +1000,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.05851099999999931</v>
+        <v>0.04446200000000111</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1008,7 +1008,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.03750800000000076</v>
+        <v>0.04460400000000142</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1016,7 +1016,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0.04416499999999957</v>
+        <v>0.04427300000000045</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1024,7 +1024,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.04995699999999914</v>
+        <v>0.04443900000000056</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1032,7 +1032,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0.05000599999999977</v>
+        <v>0.04428000000000054</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1040,7 +1040,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0.02814799999999984</v>
+        <v>0.04462100000000113</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1048,7 +1048,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0.02596899999999991</v>
+        <v>0.04445500000000102</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1056,7 +1056,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0.0489569999999997</v>
+        <v>0.04444900000000018</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1064,7 +1064,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.04842899999999872</v>
+        <v>0.044099000000001</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1072,7 +1072,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.05197700000000083</v>
+        <v>0.04442599999999963</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1080,7 +1080,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.06099799999999966</v>
+        <v>0.04445099999999869</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1088,7 +1088,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.04896499999999904</v>
+        <v>0.04461300000000001</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1096,7 +1096,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.07254299999999958</v>
+        <v>0.04449199999999998</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1104,7 +1104,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.03970400000000041</v>
+        <v>0.04427699999999923</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1112,7 +1112,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.05098699999999923</v>
+        <v>0.0442739999999997</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1120,7 +1120,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.005033000000000953</v>
+        <v>0.04437600000000153</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1128,7 +1128,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.06487399999999965</v>
+        <v>0.04463099999999898</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1136,7 +1136,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.03317299999999967</v>
+        <v>0.04463100000000075</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1144,7 +1144,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.06353999999999971</v>
+        <v>0.04445800000000055</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1152,7 +1152,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0.03099199999999946</v>
+        <v>0.04428200000000082</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1160,7 +1160,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0.0805429999999987</v>
+        <v>0.04453999999999958</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1168,7 +1168,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0.04441999999999879</v>
+        <v>0.04467900000000036</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1176,7 +1176,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0.03099199999999946</v>
+        <v>0.04464000000000112</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1184,7 +1184,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>0.003152000000000044</v>
+        <v>0.04447500000000026</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1192,7 +1192,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>0.07101299999999888</v>
+        <v>0.0444810000000011</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1200,7 +1200,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>0.006007000000000318</v>
+        <v>0.04428699999999886</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1208,7 +1208,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>0.06139899999999976</v>
+        <v>0.04466899999999896</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1216,7 +1216,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>0.005003000000000313</v>
+        <v>0.04434499999999986</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1224,7 +1224,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>0.04669699999999999</v>
+        <v>0.04474399999999967</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1232,7 +1232,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>0.08545100000000083</v>
+        <v>0.0686479999999996</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1240,7 +1240,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>0.04122000000000092</v>
+        <v>0.04449600000000054</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1248,7 +1248,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>0.08636699999999919</v>
+        <v>0.0444559999999985</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1256,7 +1256,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>0.03503300000000031</v>
+        <v>0.04449900000000007</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1264,7 +1264,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>0.0239729999999998</v>
+        <v>0.04432199999999931</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1272,7 +1272,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>0.04600699999999946</v>
+        <v>0.04447500000000026</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1280,7 +1280,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>0.0413490000000003</v>
+        <v>0.04448799999999942</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1288,7 +1288,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>0.01901600000000059</v>
+        <v>0.04446399999999961</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1296,7 +1296,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>0.08258900000000047</v>
+        <v>0.04448200000000035</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1304,7 +1304,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>0.08359199999999944</v>
+        <v>0.04444499999999962</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1312,7 +1312,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>0.05415500000000151</v>
+        <v>0.04448799999999942</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1320,7 +1320,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>0.03402300000000125</v>
+        <v>0.04465699999999906</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1328,7 +1328,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>0.05806199999999961</v>
+        <v>0.0229929999999996</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1336,7 +1336,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>0.02003200000000049</v>
+        <v>0.0445050000000009</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1344,7 +1344,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>0.07957999999999998</v>
+        <v>0.0442859999999996</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1352,7 +1352,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>0.01384299999999961</v>
+        <v>0.04449100000000072</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1360,7 +1360,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>0.07404999999999973</v>
+        <v>0.04466099999999962</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1368,7 +1368,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>0.05041000000000118</v>
+        <v>0.04466599999999943</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1376,7 +1376,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>0.07358200000000004</v>
+        <v>0.04453800000000108</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1384,7 +1384,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>0.02531900000000142</v>
+        <v>0.04430200000000006</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1392,7 +1392,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>0.04460399999999964</v>
+        <v>0.04452000000000034</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1400,7 +1400,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>0.04381899999999916</v>
+        <v>0.04420999999999964</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1408,7 +1408,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>0.01900299999999966</v>
+        <v>0.04447900000000082</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1416,7 +1416,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>0.04603799999999936</v>
+        <v>0.04431799999999875</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1424,7 +1424,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>0.02601600000000026</v>
+        <v>0.04467200000000027</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1432,7 +1432,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>0.04504999999999981</v>
+        <v>0.04462700000000019</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1440,7 +1440,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>0.0499609999999997</v>
+        <v>0.04450600000000016</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1448,7 +1448,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>0.06201199999999929</v>
+        <v>0.04469600000000007</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1456,7 +1456,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>0.05561900000000009</v>
+        <v>0.04455899999999957</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1464,7 +1464,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>0.07002099999999878</v>
+        <v>0.04453900000000033</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1472,7 +1472,7 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>0.06098099999999995</v>
+        <v>0.04456099999999985</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1480,7 +1480,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>0.02099499999999921</v>
+        <v>0.04472599999999893</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1488,7 +1488,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>0.04464600000000019</v>
+        <v>0.04450000000000109</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1496,7 +1496,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>0.0268979999999992</v>
+        <v>0.0443409999999993</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1504,7 +1504,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>0.03620800000000024</v>
+        <v>0.04451599999999978</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1512,7 +1512,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>0.04463599999999879</v>
+        <v>0.04453099999999921</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1520,7 +1520,7 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>0.0753269999999997</v>
+        <v>0.04452900000000071</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1528,7 +1528,7 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>0.05998199999999976</v>
+        <v>0.044238</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1536,7 +1536,7 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>0.05872399999999978</v>
+        <v>0.04449400000000026</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1544,7 +1544,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>0.03003099999999925</v>
+        <v>0.0445259999999994</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1552,7 +1552,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>0.05301199999999895</v>
+        <v>0.04456899999999919</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1560,7 +1560,7 @@
         <v>147</v>
       </c>
       <c r="B149">
-        <v>0.0824410000000011</v>
+        <v>0.04471399999999903</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1568,7 +1568,7 @@
         <v>148</v>
       </c>
       <c r="B150">
-        <v>0.01986499999999936</v>
+        <v>0.04472399999999865</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1576,7 +1576,7 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>0.05705799999999961</v>
+        <v>0.04469699999999932</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1584,7 +1584,7 @@
         <v>150</v>
       </c>
       <c r="B152">
-        <v>0.05899600000000049</v>
+        <v>0.04455200000000126</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1592,7 +1592,7 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>0.01202199999999998</v>
+        <v>0.04471300000000156</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1600,7 +1600,7 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>0.07732700000000037</v>
+        <v>0.04454599999999864</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1608,7 +1608,7 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>0.009763000000001298</v>
+        <v>0.04478899999999975</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1616,7 +1616,7 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>0.01999299999999948</v>
+        <v>0.04456700000000069</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1624,7 +1624,7 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>0.01821500000000142</v>
+        <v>0.04473899999999986</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1632,7 +1632,7 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>0.04529400000000194</v>
+        <v>0.04447599999999952</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1640,7 +1640,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>0.04423399999999944</v>
+        <v>0.04434799999999939</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1648,7 +1648,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>0.05601400000000112</v>
+        <v>0.04457999999999984</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1656,7 +1656,7 @@
         <v>159</v>
       </c>
       <c r="B161">
-        <v>0.03701500000000024</v>
+        <v>0.04437599999999975</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1664,7 +1664,7 @@
         <v>160</v>
       </c>
       <c r="B162">
-        <v>0.03006200000000092</v>
+        <v>0.04455199999999948</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1672,7 +1672,7 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>0.01702300000000179</v>
+        <v>0.04478599999999844</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1680,7 +1680,7 @@
         <v>162</v>
       </c>
       <c r="B164">
-        <v>0.02703899999999848</v>
+        <v>0.04477899999999835</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1688,7 +1688,7 @@
         <v>163</v>
       </c>
       <c r="B165">
-        <v>0.04420399999999702</v>
+        <v>0.04417499999999919</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1696,7 +1696,7 @@
         <v>164</v>
       </c>
       <c r="B166">
-        <v>0.06200199999999967</v>
+        <v>0.04429400000000072</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1704,7 +1704,7 @@
         <v>165</v>
       </c>
       <c r="B167">
-        <v>0.05399399999999943</v>
+        <v>0.04436600000000013</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1712,7 +1712,7 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>0.01903800000000189</v>
+        <v>0.04471799999999959</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1720,7 +1720,7 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>0.06347600000000142</v>
+        <v>0.04459400000000002</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1728,7 +1728,7 @@
         <v>168</v>
       </c>
       <c r="B170">
-        <v>0.03406500000000179</v>
+        <v>0.04450700000000296</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1736,7 +1736,7 @@
         <v>169</v>
       </c>
       <c r="B171">
-        <v>0.02699799999999897</v>
+        <v>0.0446869999999997</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1744,7 +1744,7 @@
         <v>170</v>
       </c>
       <c r="B172">
-        <v>0.02103599999999872</v>
+        <v>0.04456400000000116</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1752,7 +1752,7 @@
         <v>171</v>
       </c>
       <c r="B173">
-        <v>0.00805300000000031</v>
+        <v>0.04475200000000257</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1760,7 +1760,7 @@
         <v>172</v>
       </c>
       <c r="B174">
-        <v>0.09202600000000061</v>
+        <v>0.04443099999999944</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1768,7 +1768,7 @@
         <v>173</v>
       </c>
       <c r="B175">
-        <v>0.0572390000000027</v>
+        <v>0.04463200000000001</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1776,7 +1776,7 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>0.008012000000000796</v>
+        <v>0.04440299999999908</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1784,7 +1784,7 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>0.02332999999999785</v>
+        <v>0.04452200000000062</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1792,7 +1792,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>0.03230399999999989</v>
+        <v>0.04458699999999993</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1800,7 +1800,7 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>0.0440209999999972</v>
+        <v>0.04457899999999881</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1808,7 +1808,7 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>0.03988000000000014</v>
+        <v>0.04474000000000089</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1816,7 +1816,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>0.07124900000000167</v>
+        <v>0.04447599999999952</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1824,7 +1824,7 @@
         <v>180</v>
       </c>
       <c r="B182">
-        <v>0.04449100000000072</v>
+        <v>0.04466599999999943</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1832,7 +1832,7 @@
         <v>181</v>
       </c>
       <c r="B183">
-        <v>0.005023999999998807</v>
+        <v>0.04455099999999845</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1840,7 +1840,7 @@
         <v>182</v>
       </c>
       <c r="B184">
-        <v>0.06828399999999846</v>
+        <v>0.04473800000000239</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1848,7 +1848,7 @@
         <v>183</v>
       </c>
       <c r="B185">
-        <v>0.04470999999999847</v>
+        <v>0.04475400000000107</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1856,7 +1856,7 @@
         <v>184</v>
       </c>
       <c r="B186">
-        <v>0.05368499999999798</v>
+        <v>0.04459200000000152</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1864,7 +1864,7 @@
         <v>185</v>
       </c>
       <c r="B187">
-        <v>0.03599900000000034</v>
+        <v>0.04440400000000011</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1872,7 +1872,7 @@
         <v>186</v>
       </c>
       <c r="B188">
-        <v>0.04469800000000035</v>
+        <v>0.04439800000000105</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1880,7 +1880,7 @@
         <v>187</v>
       </c>
       <c r="B189">
-        <v>0.01540200000000169</v>
+        <v>0.04459099999999694</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1888,7 +1888,7 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>0.04000600000000176</v>
+        <v>0.04474100000000192</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1896,7 +1896,7 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>0.06512899999999888</v>
+        <v>0.04459100000000049</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1904,7 +1904,7 @@
         <v>190</v>
       </c>
       <c r="B192">
-        <v>0.04455499999999901</v>
+        <v>0.04440699999999964</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1912,7 +1912,7 @@
         <v>191</v>
       </c>
       <c r="B193">
-        <v>0.004014999999998992</v>
+        <v>0.04446299999999681</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1920,7 +1920,7 @@
         <v>192</v>
       </c>
       <c r="B194">
-        <v>0.004024000000001138</v>
+        <v>0.04477600000000237</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1928,7 +1928,7 @@
         <v>193</v>
       </c>
       <c r="B195">
-        <v>0.01904099999999787</v>
+        <v>0.04477300000000284</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1936,7 +1936,7 @@
         <v>194</v>
       </c>
       <c r="B196">
-        <v>0.05918499999999938</v>
+        <v>0.04462699999999842</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1944,7 +1944,7 @@
         <v>195</v>
       </c>
       <c r="B197">
-        <v>0.03100399999999937</v>
+        <v>0.04451899999999753</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1952,7 +1952,7 @@
         <v>196</v>
       </c>
       <c r="B198">
-        <v>0.04218399999999889</v>
+        <v>0.04460199999999759</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1960,7 +1960,7 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>0.03201599999999871</v>
+        <v>0.04441499999999721</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1968,7 +1968,7 @@
         <v>198</v>
       </c>
       <c r="B200">
-        <v>0.04299499999999767</v>
+        <v>0.04470399999999941</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -1976,7 +1976,7 @@
         <v>199</v>
       </c>
       <c r="B201">
-        <v>0.04454300000000089</v>
+        <v>0.07836200000000204</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -1984,7 +1984,7 @@
         <v>200</v>
       </c>
       <c r="B202">
-        <v>0.0430160000000015</v>
+        <v>0.04447799999999802</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -1992,7 +1992,7 @@
         <v>201</v>
       </c>
       <c r="B203">
-        <v>0.04698899999999995</v>
+        <v>0.04477999999999938</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2000,7 +2000,7 @@
         <v>202</v>
       </c>
       <c r="B204">
-        <v>0.03521500000000088</v>
+        <v>0.04485899999999887</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2008,7 +2008,7 @@
         <v>203</v>
       </c>
       <c r="B205">
-        <v>0.06712500000000077</v>
+        <v>0.04459300000000255</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2016,7 +2016,7 @@
         <v>204</v>
       </c>
       <c r="B206">
-        <v>0.07152499999999762</v>
+        <v>0.04462499999999991</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2024,7 +2024,7 @@
         <v>205</v>
       </c>
       <c r="B207">
-        <v>0.01703499999999991</v>
+        <v>0.0446040000000032</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2032,7 +2032,7 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>0.05921599999999927</v>
+        <v>0.04441399999999973</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2040,7 +2040,7 @@
         <v>207</v>
       </c>
       <c r="B209">
-        <v>0.01803499999999758</v>
+        <v>0.04451900000000109</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2048,7 +2048,7 @@
         <v>208</v>
       </c>
       <c r="B210">
-        <v>0.01902400000000171</v>
+        <v>0.04469699999999932</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2056,7 +2056,7 @@
         <v>209</v>
       </c>
       <c r="B211">
-        <v>0.06253000000000242</v>
+        <v>0.04478500000000096</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2064,7 +2064,7 @@
         <v>210</v>
       </c>
       <c r="B212">
-        <v>0.03099900000000133</v>
+        <v>0.04479700000000264</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2072,7 +2072,7 @@
         <v>211</v>
       </c>
       <c r="B213">
-        <v>0.08468299999999829</v>
+        <v>0.04461600000000132</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2080,7 +2080,7 @@
         <v>212</v>
       </c>
       <c r="B214">
-        <v>0.06754899999999964</v>
+        <v>0.04463799999999907</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2088,7 +2088,7 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>0.01502900000000196</v>
+        <v>0.04477799999999732</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2096,7 +2096,7 @@
         <v>214</v>
       </c>
       <c r="B216">
-        <v>0.05300199999999933</v>
+        <v>0.04432800000000015</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2104,7 +2104,7 @@
         <v>215</v>
       </c>
       <c r="B217">
-        <v>0.0360180000000021</v>
+        <v>0.04445000000000121</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2112,7 +2112,7 @@
         <v>216</v>
       </c>
       <c r="B218">
-        <v>0.01597799999999694</v>
+        <v>0.04444099999999906</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2120,7 +2120,7 @@
         <v>217</v>
       </c>
       <c r="B219">
-        <v>0.02003700000000208</v>
+        <v>0.04462600000000094</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2128,7 +2128,7 @@
         <v>218</v>
       </c>
       <c r="B220">
-        <v>0.06069700000000111</v>
+        <v>0.04479999999999862</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2136,7 +2136,7 @@
         <v>219</v>
       </c>
       <c r="B221">
-        <v>0.07315700000000191</v>
+        <v>0.04462399999999889</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2144,7 +2144,7 @@
         <v>220</v>
       </c>
       <c r="B222">
-        <v>0.03519100000000108</v>
+        <v>0.04452699999999865</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2152,7 +2152,7 @@
         <v>221</v>
       </c>
       <c r="B223">
-        <v>0.07201200000000085</v>
+        <v>0.04478500000000096</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2160,7 +2160,7 @@
         <v>222</v>
       </c>
       <c r="B224">
-        <v>0.04457599999999928</v>
+        <v>0.04463799999999907</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2168,7 +2168,7 @@
         <v>223</v>
       </c>
       <c r="B225">
-        <v>0.04458299999999937</v>
+        <v>0.04478500000000096</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2176,7 +2176,7 @@
         <v>224</v>
       </c>
       <c r="B226">
-        <v>0.04484399999999766</v>
+        <v>0.04464400000000168</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2184,7 +2184,7 @@
         <v>225</v>
       </c>
       <c r="B227">
-        <v>0.04458300000000293</v>
+        <v>0.04453099999999921</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2192,7 +2192,7 @@
         <v>226</v>
       </c>
       <c r="B228">
-        <v>0.08300300000000149</v>
+        <v>0.04431500000000099</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2200,7 +2200,7 @@
         <v>227</v>
       </c>
       <c r="B229">
-        <v>0.04917099999999763</v>
+        <v>0.04463800000000262</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2208,7 +2208,7 @@
         <v>228</v>
       </c>
       <c r="B230">
-        <v>0.06359299999999735</v>
+        <v>0.04479299999999853</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -2216,7 +2216,7 @@
         <v>229</v>
       </c>
       <c r="B231">
-        <v>0.04457800000000134</v>
+        <v>0.04463299999999748</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -2224,7 +2224,7 @@
         <v>230</v>
       </c>
       <c r="B232">
-        <v>0.08460499999999982</v>
+        <v>0.04446899999999943</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -2232,7 +2232,7 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>0.0448270000000015</v>
+        <v>0.04467400000000055</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2240,7 +2240,7 @@
         <v>232</v>
       </c>
       <c r="B234">
-        <v>0.03296399999999977</v>
+        <v>0.04424700000000215</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -2248,7 +2248,7 @@
         <v>233</v>
       </c>
       <c r="B235">
-        <v>0.04316299999999984</v>
+        <v>0.04482400000000197</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -2256,7 +2256,7 @@
         <v>234</v>
       </c>
       <c r="B236">
-        <v>0.03150999999999726</v>
+        <v>0.04462699999999842</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -2264,7 +2264,7 @@
         <v>235</v>
       </c>
       <c r="B237">
-        <v>0.05576900000000151</v>
+        <v>0.04485299999999981</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -2272,7 +2272,7 @@
         <v>236</v>
       </c>
       <c r="B238">
-        <v>0.04469900000000138</v>
+        <v>0.04464199999999963</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2280,7 +2280,7 @@
         <v>237</v>
       </c>
       <c r="B239">
-        <v>0.07955799999999869</v>
+        <v>0.04457700000000031</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2288,7 +2288,7 @@
         <v>238</v>
       </c>
       <c r="B240">
-        <v>0.05199599999999904</v>
+        <v>0.04485500000000187</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2296,7 +2296,7 @@
         <v>239</v>
       </c>
       <c r="B241">
-        <v>0.04456399999999761</v>
+        <v>0.04484799999999822</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2304,7 +2304,7 @@
         <v>240</v>
       </c>
       <c r="B242">
-        <v>0.04460299999999862</v>
+        <v>0.04446599999999989</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -2312,7 +2312,7 @@
         <v>241</v>
       </c>
       <c r="B243">
-        <v>0.02903200000000083</v>
+        <v>0.04466600000000298</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -2320,7 +2320,7 @@
         <v>242</v>
       </c>
       <c r="B244">
-        <v>0.05199499999999802</v>
+        <v>0.04444400000000215</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -2328,7 +2328,7 @@
         <v>243</v>
       </c>
       <c r="B245">
-        <v>0.0190659999999987</v>
+        <v>0.04489699999999885</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -2336,7 +2336,7 @@
         <v>244</v>
       </c>
       <c r="B246">
-        <v>0.03396100000000146</v>
+        <v>0.04467299999999952</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -2344,7 +2344,7 @@
         <v>245</v>
       </c>
       <c r="B247">
-        <v>0.04797299999999893</v>
+        <v>0.04453499999999977</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -2352,7 +2352,7 @@
         <v>246</v>
       </c>
       <c r="B248">
-        <v>0.05535800000000179</v>
+        <v>0.04445699999999775</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -2360,7 +2360,7 @@
         <v>247</v>
       </c>
       <c r="B249">
-        <v>0.04517600000000144</v>
+        <v>0.04466400000000093</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -2368,7 +2368,7 @@
         <v>248</v>
       </c>
       <c r="B250">
-        <v>0.05304800000000043</v>
+        <v>0.04481700000000188</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -2376,7 +2376,7 @@
         <v>249</v>
       </c>
       <c r="B251">
-        <v>0.0447810000000004</v>
+        <v>0.04486500000000149</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -2384,7 +2384,7 @@
         <v>250</v>
       </c>
       <c r="B252">
-        <v>0.07959200000000166</v>
+        <v>0.04466599999999943</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -2392,7 +2392,7 @@
         <v>251</v>
       </c>
       <c r="B253">
-        <v>0.07776099999999886</v>
+        <v>0.04467599999999905</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -2400,7 +2400,7 @@
         <v>252</v>
       </c>
       <c r="B254">
-        <v>0.04478699999999947</v>
+        <v>0.04448499999999811</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -2408,7 +2408,7 @@
         <v>253</v>
       </c>
       <c r="B255">
-        <v>0.05718200000000095</v>
+        <v>0.04484500000000224</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -2416,7 +2416,7 @@
         <v>254</v>
       </c>
       <c r="B256">
-        <v>0.01501400000000075</v>
+        <v>0.04468299999999914</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -2424,7 +2424,7 @@
         <v>255</v>
       </c>
       <c r="B257">
-        <v>0.0270229999999998</v>
+        <v>0.04431500000000099</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -2432,7 +2432,7 @@
         <v>256</v>
       </c>
       <c r="B258">
-        <v>0.02904400000000251</v>
+        <v>0.0446760000000026</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -2440,7 +2440,7 @@
         <v>257</v>
       </c>
       <c r="B259">
-        <v>0.04598800000000125</v>
+        <v>0.04450399999999988</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -2448,7 +2448,7 @@
         <v>258</v>
       </c>
       <c r="B260">
-        <v>0.006040999999999741</v>
+        <v>0.04487599999999858</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -2456,7 +2456,7 @@
         <v>259</v>
       </c>
       <c r="B261">
-        <v>0.07230500000000006</v>
+        <v>0.04466700000000046</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -2464,7 +2464,7 @@
         <v>260</v>
       </c>
       <c r="B262">
-        <v>0.003970999999999947</v>
+        <v>0.04473099999999874</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -2472,7 +2472,7 @@
         <v>261</v>
       </c>
       <c r="B263">
-        <v>0.05618300000000076</v>
+        <v>0.04486400000000046</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -2480,7 +2480,7 @@
         <v>262</v>
       </c>
       <c r="B264">
-        <v>0.08525900000000064</v>
+        <v>0.04485899999999887</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -2488,7 +2488,7 @@
         <v>263</v>
       </c>
       <c r="B265">
-        <v>0.05130400000000179</v>
+        <v>0.04466800000000148</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -2496,7 +2496,7 @@
         <v>264</v>
       </c>
       <c r="B266">
-        <v>0.01403700000000185</v>
+        <v>0.04470099999999988</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -2504,7 +2504,7 @@
         <v>265</v>
       </c>
       <c r="B267">
-        <v>0.05279799999999923</v>
+        <v>0.0446869999999997</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -2512,7 +2512,7 @@
         <v>266</v>
       </c>
       <c r="B268">
-        <v>0.04311799999999977</v>
+        <v>0.04461200000000076</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -2520,7 +2520,7 @@
         <v>267</v>
       </c>
       <c r="B269">
-        <v>0.01618799999999965</v>
+        <v>0.035026000000002</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -2528,7 +2528,7 @@
         <v>268</v>
       </c>
       <c r="B270">
-        <v>0.06620899999999708</v>
+        <v>0.04485599999999934</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2536,7 +2536,7 @@
         <v>269</v>
       </c>
       <c r="B271">
-        <v>0.04798499999999706</v>
+        <v>0.04485200000000233</v>
       </c>
     </row>
   </sheetData>
@@ -2562,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.04333232592592585</v>
+        <v>44.68041111111113</v>
       </c>
     </row>
   </sheetData>
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.007352941176470588</v>
+        <v>0.7352941176470589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>